<commit_message>
membuat perbaikan dan penyesuaian pada model dan controller karena perubahan struktur database
</commit_message>
<xml_diff>
--- a/public/format-kolom/Format Kolom Petugas.xlsx
+++ b/public/format-kolom/Format Kolom Petugas.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ApkLaravel\direktori-perusahaan-kota-medan\public\format-kolom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Blok 1-3.xlsx - import_petugas" sheetId="1" r:id="rId1"/>
+    <sheet name="format_petugas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>email</t>
   </si>
@@ -33,6 +33,9 @@
     <t>nama_petugas</t>
   </si>
   <si>
+    <t>kode_kegiatan</t>
+  </si>
+  <si>
     <t>jenis_kelamin</t>
   </si>
   <si>
@@ -45,7 +48,7 @@
     <t>alamat</t>
   </si>
   <si>
-    <t>petugas11@gmail.com</t>
+    <t>petugas13@gmail.com</t>
   </si>
   <si>
     <t>id11</t>
@@ -54,13 +57,16 @@
     <t>petugas11</t>
   </si>
   <si>
+    <t>sk04</t>
+  </si>
+  <si>
     <t>laki-laki</t>
   </si>
   <si>
     <t>Jl.Helvetia</t>
   </si>
   <si>
-    <t>petugas12@gmail.com</t>
+    <t>petugas14@gmail.com</t>
   </si>
   <si>
     <t>id12</t>
@@ -69,10 +75,13 @@
     <t>petugas12</t>
   </si>
   <si>
+    <t>sk05</t>
+  </si>
+  <si>
     <t>perempuan</t>
   </si>
   <si>
-    <t>petugas13@gmail.com</t>
+    <t>petugas15@gmail.com</t>
   </si>
   <si>
     <t>id13</t>
@@ -81,7 +90,10 @@
     <t>petugas13</t>
   </si>
   <si>
-    <t>petugas14@gmail.com</t>
+    <t>sk06</t>
+  </si>
+  <si>
+    <t>petugas16@gmail.com</t>
   </si>
   <si>
     <t>id14</t>
@@ -90,23 +102,20 @@
     <t>petugas14</t>
   </si>
   <si>
-    <t>853900821202</t>
-  </si>
-  <si>
-    <t>853900821203</t>
-  </si>
-  <si>
-    <t>853900821201</t>
-  </si>
-  <si>
-    <t>853900821204</t>
+    <t>petugas17@gmail.com</t>
+  </si>
+  <si>
+    <t>id15</t>
+  </si>
+  <si>
+    <t>petugas15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +250,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF047857"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,8 +437,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1FAE5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -538,6 +559,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -583,9 +619,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -907,18 +946,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -943,112 +982,157 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
         <v>34</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1">
+        <v>853900821201</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1">
+        <v>853900821202</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1">
+        <v>853900821203</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1">
+        <v>853900821204</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G6">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1">
+        <v>853900821205</v>
+      </c>
+      <c r="I6" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <v>35</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>36</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5">
-        <v>37</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>